<commit_message>
Updated the trials spreadsheet
The sheet now accounts for the checkout page and has documented the changes in the cart page
</commit_message>
<xml_diff>
--- a/Trials.xlsx
+++ b/Trials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlantictu-my.sharepoint.com/personal/g00417466_atu_ie/Documents/Java Labs 2022/User Interface, Web Development/DnD-Retailer Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlantictu-my.sharepoint.com/personal/g00417466_atu_ie/Documents/Java Labs 2022/User Interface, Web Development/DnD-Retailer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F3852DF-B7AD-4808-9D9E-7072FA548E45}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92A3A552-9FF6-4E79-AC36-C39EED30A621}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t xml:space="preserve">TEST CASES: </t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>Changed the storage from session to local storage</t>
+  </si>
+  <si>
+    <t>Checkout Button(Trial 2)</t>
+  </si>
+  <si>
+    <t>Brings user to the checkout page</t>
+  </si>
+  <si>
+    <t>Button now saves user data and brings them to the checkout page</t>
+  </si>
+  <si>
+    <t>CHECKOUT PAGE</t>
+  </si>
+  <si>
+    <t>Checkout button</t>
+  </si>
+  <si>
+    <t>Take user info and complete transaction</t>
   </si>
 </sst>
 </file>
@@ -459,16 +477,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K32"/>
+  <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="69.42578125" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
@@ -621,83 +639,86 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>20</v>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>11</v>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -705,64 +726,105 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
         <v>10</v>
       </c>
-      <c r="E28" t="s">
-        <v>35</v>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>11</v>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C37" t="s">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D37" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>